<commit_message>
official grading sent out
</commit_message>
<xml_diff>
--- a/Adm/unix_score.xlsx
+++ b/Adm/unix_score.xlsx
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>